<commit_message>
Fixed small bugs in the code related to balance summary calculations
</commit_message>
<xml_diff>
--- a/ollama/categorized_data.xlsx
+++ b/ollama/categorized_data.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D179"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4006,6 +4006,286 @@
         </is>
       </c>
       <c r="D179" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>12/20/2023</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>104</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Employer</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>12/15/2023</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>11/30/2023</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>11/27/2023</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>300</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>11/22/2023</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>104</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Employer</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>11/22/2023</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>200</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>10/31/2023</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>300</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>American Heritage</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>10/20/2023</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>100</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>From Share 00</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>10/10/2023</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>54</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>From Share 00</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>12/15/2023</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>11/30/2023</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>11/29/2023</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>210</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>From Share 00</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>11/27/2023</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>300</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>11/22/2023</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>200</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>TIJO VARUGHESE : P2P PAYMNT  ID: 9000041902CO: American Heritag  NAME: TIJO VARUGHESE %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
         <is>
           <t>Upwork</t>
         </is>
@@ -4022,7 +4302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D642"/>
+  <dimension ref="A1:D643"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16869,6 +17149,26 @@
       <c r="D642" t="inlineStr">
         <is>
           <t>Employer</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>11/29/2023</t>
+        </is>
+      </c>
+      <c r="B643" t="n">
+        <v>15</v>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>ODP Fee %% ACH ECC WEB %% ACH Trace 091000016840533</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>Bank</t>
         </is>
       </c>
     </row>
@@ -16883,7 +17183,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D275"/>
+  <dimension ref="A1:D289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22390,6 +22690,286 @@
       <c r="D275" t="inlineStr">
         <is>
           <t>Upwork</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>12/29/2023</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>85</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Business Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>12/18/2023</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>2861</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Business Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>11/29/2023</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>954</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Business Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>11/13/2023</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>120</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>11/02/2023</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>105</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>10/20/2023</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>100</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>10/10/2023</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>105</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>10/10/2023</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>35</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>09/14/2023</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>14</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>FIVERR INTERNATI CO: FIVERR INTERNATIONAL LTD. : IAT PAYPAL  ID: 770510487C DATA: FF3               US</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Fiverr</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>12/29/2023</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>85</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Business Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>12/20/2023</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>104</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Employer</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>12/18/2023</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>2861</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES %% ACH ECC WEB</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Business Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>11/29/2023</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>954</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>PAYPAL : INST XFER  ID: PAYPALSI77 DATA: INSTANT TRANSFER  CO: PAYPAL NAME: CREED SERVICES</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Business Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>11/22/2023</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>104</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>PATRICK RIVERA CO: PATRICK RIVERA : IAT PAYPAL  ID: 770510487C DATA: FF3               US %% ACH ECC IAT</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Employer</t>
         </is>
       </c>
     </row>
@@ -22505,7 +23085,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22852,6 +23432,66 @@
       <c r="D17" t="inlineStr">
         <is>
           <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>09/06/2023</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>37</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>INSTANTLY.AI SHERIDAN US  09/05/23%% Card 15 #9560</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Instantly.ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08/06/2023</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>37</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>INSTANTLY.AI SHERIDAN US  08/05/23%% Card 15 #9560</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Instantly.ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>37</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>INSTANTLY.AI SHERIDAN US  07/05/23%% Card 15 #9560</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Instantly.ai</t>
         </is>
       </c>
     </row>
@@ -22866,7 +23506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23223,6 +23863,86 @@
       <c r="D19" t="inlineStr">
         <is>
           <t>Uncertain</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>12/13/2023</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>To Share 00 REF# 30479632</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>11/29/2023</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>15</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ODP Fee %% ACH ECC WEB %% ACH Trace 091000016840533</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11/29/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>210</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>From Share 00</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>12/13/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>To Share 00 REF# 30479632</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Bank</t>
         </is>
       </c>
     </row>
@@ -23237,7 +23957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23270,855 +23990,861 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01/02/23</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>334109</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-334109</v>
+          <t>Week Start</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01/09/23</t>
+          <t>01/02/23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13118</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>5901</v>
+        <v>334109</v>
       </c>
       <c r="D3" t="n">
-        <v>7217</v>
+        <v>-334109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01/16/23</t>
+          <t>01/09/23</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>13118</v>
       </c>
       <c r="C4" t="n">
-        <v>952</v>
+        <v>5901</v>
       </c>
       <c r="D4" t="n">
-        <v>-952</v>
+        <v>7217</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>01/23/23</t>
+          <t>01/16/23</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4161</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>6477</v>
+        <v>952</v>
       </c>
       <c r="D5" t="n">
-        <v>-2316</v>
+        <v>-952</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01/30/23</t>
+          <t>01/23/23</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1686.02</v>
+        <v>4161</v>
       </c>
       <c r="C6" t="n">
-        <v>8463</v>
+        <v>6477</v>
       </c>
       <c r="D6" t="n">
-        <v>-6776.98</v>
+        <v>-2316</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02/06/23</t>
+          <t>01/30/23</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>14163</v>
+        <v>1686.02</v>
       </c>
       <c r="C7" t="n">
-        <v>48870</v>
+        <v>8463</v>
       </c>
       <c r="D7" t="n">
-        <v>-34707</v>
+        <v>-6776.98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02/13/23</t>
+          <t>02/06/23</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>14163</v>
       </c>
       <c r="C8" t="n">
-        <v>2107</v>
+        <v>48870</v>
       </c>
       <c r="D8" t="n">
-        <v>-2107</v>
+        <v>-34707</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02/20/23</t>
+          <t>02/13/23</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3927</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>8856</v>
+        <v>2107</v>
       </c>
       <c r="D9" t="n">
-        <v>-4929</v>
+        <v>-2107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>02/27/23</t>
+          <t>02/20/23</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>761.02</v>
+        <v>3927</v>
       </c>
       <c r="C10" t="n">
-        <v>33565</v>
+        <v>8856</v>
       </c>
       <c r="D10" t="n">
-        <v>-32803.98</v>
+        <v>-4929</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/06/23</t>
+          <t>02/27/23</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4058</v>
+        <v>761.02</v>
       </c>
       <c r="C11" t="n">
-        <v>16293</v>
+        <v>33565</v>
       </c>
       <c r="D11" t="n">
-        <v>-12235</v>
+        <v>-32803.98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/13/23</t>
+          <t>03/06/23</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1099</v>
+        <v>4058</v>
       </c>
       <c r="C12" t="n">
-        <v>1269</v>
+        <v>16345</v>
       </c>
       <c r="D12" t="n">
-        <v>-170</v>
+        <v>-12287</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/20/23</t>
+          <t>03/13/23</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3927</v>
+        <v>1099</v>
       </c>
       <c r="C13" t="n">
-        <v>4711</v>
+        <v>1269</v>
       </c>
       <c r="D13" t="n">
-        <v>-784</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/27/23</t>
+          <t>03/20/23</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1421</v>
+        <v>3927</v>
       </c>
       <c r="C14" t="n">
-        <v>28812</v>
+        <v>4711</v>
       </c>
       <c r="D14" t="n">
-        <v>-27391</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04/03/23</t>
+          <t>03/27/23</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>150</v>
+        <v>1421</v>
       </c>
       <c r="C15" t="n">
-        <v>854</v>
+        <v>28812</v>
       </c>
       <c r="D15" t="n">
-        <v>-704</v>
+        <v>-27391</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04/10/23</t>
+          <t>04/03/23</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C16" t="n">
-        <v>4996</v>
+        <v>854</v>
       </c>
       <c r="D16" t="n">
-        <v>-4856</v>
+        <v>-704</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04/17/23</t>
+          <t>04/10/23</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8649</v>
+        <v>140</v>
       </c>
       <c r="C17" t="n">
-        <v>6111</v>
+        <v>5021</v>
       </c>
       <c r="D17" t="n">
-        <v>2538</v>
+        <v>-4881</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04/24/23</t>
+          <t>04/17/23</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1632</v>
+        <v>8649</v>
       </c>
       <c r="C18" t="n">
-        <v>13512</v>
+        <v>6111</v>
       </c>
       <c r="D18" t="n">
-        <v>-11880</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05/01/23</t>
+          <t>04/24/23</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4258</v>
+        <v>1632</v>
       </c>
       <c r="C19" t="n">
-        <v>7325</v>
+        <v>13512</v>
       </c>
       <c r="D19" t="n">
-        <v>-3067</v>
+        <v>-11880</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05/08/23</t>
+          <t>05/01/23</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>108</v>
+        <v>4258</v>
       </c>
       <c r="C20" t="n">
-        <v>706</v>
+        <v>7325</v>
       </c>
       <c r="D20" t="n">
-        <v>-598</v>
+        <v>-3067</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05/15/23</t>
+          <t>05/08/23</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4584</v>
+        <v>215</v>
       </c>
       <c r="C21" t="n">
-        <v>1377</v>
+        <v>889</v>
       </c>
       <c r="D21" t="n">
-        <v>3207</v>
+        <v>-674</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05/22/23</t>
+          <t>05/15/23</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>24</v>
+        <v>4584</v>
       </c>
       <c r="C22" t="n">
-        <v>779</v>
+        <v>1377</v>
       </c>
       <c r="D22" t="n">
-        <v>-755</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05/29/23</t>
+          <t>05/22/23</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5717</v>
+        <v>24</v>
       </c>
       <c r="C23" t="n">
-        <v>11108</v>
+        <v>779</v>
       </c>
       <c r="D23" t="n">
-        <v>-5391</v>
+        <v>-755</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06/05/23</t>
+          <t>05/29/23</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>8418</v>
+        <v>5717</v>
       </c>
       <c r="C24" t="n">
-        <v>5050</v>
+        <v>11108</v>
       </c>
       <c r="D24" t="n">
-        <v>3368</v>
+        <v>-5391</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>06/12/23</t>
+          <t>06/05/23</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4558</v>
+        <v>8418</v>
       </c>
       <c r="C25" t="n">
-        <v>5067</v>
+        <v>5050</v>
       </c>
       <c r="D25" t="n">
-        <v>-509</v>
+        <v>3368</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06/19/23</t>
+          <t>06/12/23</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3000</v>
+        <v>4558</v>
       </c>
       <c r="C26" t="n">
-        <v>1033</v>
+        <v>5067</v>
       </c>
       <c r="D26" t="n">
-        <v>1967</v>
+        <v>-509</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06/26/23</t>
+          <t>06/19/23</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4268</v>
+        <v>3000</v>
       </c>
       <c r="C27" t="n">
-        <v>10280</v>
+        <v>1033</v>
       </c>
       <c r="D27" t="n">
-        <v>-6012</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07/03/23</t>
+          <t>06/26/23</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3927</v>
+        <v>4268</v>
       </c>
       <c r="C28" t="n">
-        <v>4628</v>
+        <v>10280</v>
       </c>
       <c r="D28" t="n">
-        <v>-701</v>
+        <v>-6012</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07/10/23</t>
+          <t>07/03/23</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>7810</v>
+        <v>3927</v>
       </c>
       <c r="C29" t="n">
-        <v>9433</v>
+        <v>4628</v>
       </c>
       <c r="D29" t="n">
-        <v>-1623</v>
+        <v>-701</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>07/17/23</t>
+          <t>07/10/23</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1000</v>
+        <v>7810</v>
       </c>
       <c r="C30" t="n">
-        <v>398</v>
+        <v>9433</v>
       </c>
       <c r="D30" t="n">
-        <v>602</v>
+        <v>-1623</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>07/24/23</t>
+          <t>07/17/23</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>43098.93</v>
+        <v>1000</v>
       </c>
       <c r="C31" t="n">
-        <v>511660.88</v>
+        <v>398</v>
       </c>
       <c r="D31" t="n">
-        <v>-468561.95</v>
+        <v>602</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>07/31/23</t>
+          <t>07/24/23</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>70</v>
+        <v>43098.93</v>
       </c>
       <c r="C32" t="n">
-        <v>963</v>
+        <v>511660.88</v>
       </c>
       <c r="D32" t="n">
-        <v>-893</v>
+        <v>-468561.95</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>08/07/23</t>
+          <t>07/31/23</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>6583</v>
+        <v>70</v>
       </c>
       <c r="C33" t="n">
-        <v>12964</v>
+        <v>963</v>
       </c>
       <c r="D33" t="n">
-        <v>-6381</v>
+        <v>-893</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>08/14/23</t>
+          <t>08/07/23</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>200</v>
+        <v>6583</v>
       </c>
       <c r="C34" t="n">
-        <v>5289</v>
+        <v>12964</v>
       </c>
       <c r="D34" t="n">
-        <v>-5089</v>
+        <v>-6381</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>08/21/23</t>
+          <t>08/14/23</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4071</v>
+        <v>200</v>
       </c>
       <c r="C35" t="n">
-        <v>9032</v>
+        <v>5289</v>
       </c>
       <c r="D35" t="n">
-        <v>-4961</v>
+        <v>-5089</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>08/28/23</t>
+          <t>08/21/23</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>8</v>
+        <v>4071</v>
       </c>
       <c r="C36" t="n">
-        <v>7665</v>
+        <v>9032</v>
       </c>
       <c r="D36" t="n">
-        <v>-7657</v>
+        <v>-4961</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>09/04/23</t>
+          <t>08/28/23</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1973</v>
+        <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>1621</v>
+        <v>7665</v>
       </c>
       <c r="D37" t="n">
-        <v>352</v>
+        <v>-7657</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>09/11/23</t>
+          <t>09/04/23</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>300</v>
+        <v>1973</v>
       </c>
       <c r="C38" t="n">
-        <v>3010</v>
+        <v>1621</v>
       </c>
       <c r="D38" t="n">
-        <v>-2710</v>
+        <v>352</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>09/18/23</t>
+          <t>09/11/23</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>40997</v>
+        <v>300</v>
       </c>
       <c r="C39" t="n">
-        <v>44102</v>
+        <v>3010</v>
       </c>
       <c r="D39" t="n">
-        <v>-3105</v>
+        <v>-2710</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>09/25/23</t>
+          <t>09/18/23</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>12298</v>
+        <v>40997</v>
       </c>
       <c r="C40" t="n">
-        <v>7673</v>
+        <v>44102</v>
       </c>
       <c r="D40" t="n">
-        <v>4625</v>
+        <v>-3105</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>10/02/23</t>
+          <t>09/25/23</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>8854</v>
+        <v>12298</v>
       </c>
       <c r="C41" t="n">
-        <v>10168</v>
+        <v>7673</v>
       </c>
       <c r="D41" t="n">
-        <v>-1314</v>
+        <v>4625</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>10/09/23</t>
+          <t>10/02/23</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>693</v>
+        <v>8854</v>
       </c>
       <c r="C42" t="n">
-        <v>3752</v>
+        <v>10168</v>
       </c>
       <c r="D42" t="n">
-        <v>-3059</v>
+        <v>-1314</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>10/16/23</t>
+          <t>10/09/23</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4258</v>
+        <v>747</v>
       </c>
       <c r="C43" t="n">
-        <v>7766</v>
+        <v>3752</v>
       </c>
       <c r="D43" t="n">
-        <v>-3508</v>
+        <v>-3005</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>10/23/23</t>
+          <t>10/16/23</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>4358</v>
       </c>
       <c r="C44" t="n">
-        <v>5177</v>
+        <v>7766</v>
       </c>
       <c r="D44" t="n">
-        <v>-5177</v>
+        <v>-3408</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>10/30/23</t>
+          <t>10/23/23</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>4424</v>
+        <v>5177</v>
       </c>
       <c r="D45" t="n">
-        <v>-4124</v>
+        <v>-5177</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>11/06/23</t>
+          <t>10/30/23</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7833</v>
+        <v>600</v>
       </c>
       <c r="C46" t="n">
-        <v>3153</v>
+        <v>4424</v>
       </c>
       <c r="D46" t="n">
-        <v>4680</v>
+        <v>-3824</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>11/13/23</t>
+          <t>11/06/23</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>14059</v>
+        <v>7833</v>
       </c>
       <c r="C47" t="n">
-        <v>4161</v>
+        <v>3153</v>
       </c>
       <c r="D47" t="n">
-        <v>9898</v>
+        <v>4680</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>11/20/23</t>
+          <t>11/13/23</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>200</v>
+        <v>14059</v>
       </c>
       <c r="C48" t="n">
-        <v>6682</v>
+        <v>4161</v>
       </c>
       <c r="D48" t="n">
-        <v>-6482</v>
+        <v>9898</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>11/27/23</t>
+          <t>11/20/23</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3310</v>
+        <v>704</v>
       </c>
       <c r="C49" t="n">
-        <v>18927</v>
+        <v>6786</v>
       </c>
       <c r="D49" t="n">
-        <v>-15617</v>
+        <v>-6082</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>12/04/23</t>
+          <t>11/27/23</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>455</v>
+        <v>6120</v>
       </c>
       <c r="C50" t="n">
-        <v>3352</v>
+        <v>18942</v>
       </c>
       <c r="D50" t="n">
-        <v>-2897</v>
+        <v>-12822</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>12/11/23</t>
+          <t>12/04/23</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>10274</v>
+        <v>455</v>
       </c>
       <c r="C51" t="n">
-        <v>9295</v>
+        <v>3352</v>
       </c>
       <c r="D51" t="n">
-        <v>979</v>
+        <v>-2897</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>12/18/23</t>
+          <t>12/11/23</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>200</v>
+        <v>16274</v>
       </c>
       <c r="C52" t="n">
-        <v>5291</v>
+        <v>9295</v>
       </c>
       <c r="D52" t="n">
-        <v>-5091</v>
+        <v>6979</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>12/25/23</t>
+          <t>12/18/23</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>4678</v>
+        <v>304</v>
       </c>
       <c r="C53" t="n">
-        <v>8429</v>
+        <v>5482</v>
       </c>
       <c r="D53" t="n">
-        <v>-3751</v>
+        <v>-5178</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>01/01/24</t>
+          <t>12/25/23</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>4678</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>8714</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>-4036</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>01/08/24</t>
+          <t>01/01/24</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -24134,7 +24860,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>01/15/24</t>
+          <t>01/08/24</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -24150,7 +24876,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>01/22/24</t>
+          <t>01/15/24</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -24166,7 +24892,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>01/29/24</t>
+          <t>01/22/24</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -24182,7 +24908,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>02/05/24</t>
+          <t>01/29/24</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -24198,55 +24924,55 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>02/12/24</t>
+          <t>02/05/24</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>-70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>02/19/24</t>
+          <t>02/12/24</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="D61" t="n">
-        <v>-18</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>02/26/24</t>
+          <t>02/19/24</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>03/04/24</t>
+          <t>02/26/24</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -24262,7 +24988,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>03/11/24</t>
+          <t>03/04/24</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -24278,7 +25004,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>03/18/24</t>
+          <t>03/11/24</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -24294,7 +25020,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>03/25/24</t>
+          <t>03/18/24</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -24310,32 +25036,48 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>04/01/24</t>
+          <t>03/25/24</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>860</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>-860</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>04/01/24</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>860</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-860</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>04/08/24</t>
         </is>
       </c>
-      <c r="B68" t="n">
-        <v>0</v>
-      </c>
-      <c r="C68" t="n">
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+      <c r="C69" t="n">
         <v>104</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D69" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -24395,11 +25137,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bank</t>
+          <t>bank</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>28099</v>
+        <v>3000000</v>
       </c>
     </row>
   </sheetData>
@@ -24413,7 +25155,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24450,7 +25192,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>271276.97</v>
+        <v>281255.97</v>
       </c>
     </row>
     <row r="3">
@@ -24460,7 +25202,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1092273.82</v>
+        <v>1399055.88</v>
       </c>
     </row>
     <row r="4">
@@ -24470,47 +25212,57 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-820996.8500000001</v>
+        <v>-1117799.91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Available Budget</t>
+          <t>Total Balance</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-820996.8500000001</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Daily Budget</t>
+          <t>Available Budget</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-2249.306438356165</v>
+        <v>1882200.09</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Weekly Budget</t>
+          <t>Daily Budget</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-15788.40096153846</v>
+        <v>5156.712575342466</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Weekly Budget</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>36196.15557692308</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Yearly Budget</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>-820996.8500000001</v>
+      <c r="B9" t="n">
+        <v>1882200.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>